<commit_message>
Data cleaning into driver_standings.xlsx, constructors.xlsx and drivers.xlsx files.
</commit_message>
<xml_diff>
--- a/Data xlsx/drivers.xlsx
+++ b/Data xlsx/drivers.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analysis\Formula 1\Data xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2EB47C-009B-4DA3-8448-F0B6643A6EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F4984B-F3E0-44DC-87A1-99DBC4BC6357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="drivers" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -9935,7 +9948,37 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
@@ -9962,7 +10005,7 @@
     <tableColumn id="4" xr3:uid="{6BAB627F-675D-48B4-A07A-2836C1FD98E5}" name="code"/>
     <tableColumn id="5" xr3:uid="{0DC5D08B-5039-4B89-8201-AA0FB9527FF4}" name="forename"/>
     <tableColumn id="6" xr3:uid="{DA1C872C-B043-4AAF-80F7-1591EF7BAFD3}" name="surname"/>
-    <tableColumn id="7" xr3:uid="{F00CC92A-C3B3-4F95-BF34-EB3F114ACC78}" name="dob" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{F00CC92A-C3B3-4F95-BF34-EB3F114ACC78}" name="dob" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{A60E1591-D90B-4381-B6FF-2A58B7A19CCE}" name="nationality"/>
     <tableColumn id="9" xr3:uid="{20BFF15C-36E5-4F32-8338-4B24BF6795B3}" name="url"/>
   </tableColumns>
@@ -10270,7 +10313,7 @@
   <dimension ref="A1:I858"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G861" sqref="G861"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35169,6 +35212,12 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>